<commit_message>
add print userid in top20 and fix a bug about '->A->B' miss a data
</commit_message>
<xml_diff>
--- a/21.04.14-Sequential_Pattern/三类模式Top15.xlsx
+++ b/21.04.14-Sequential_Pattern/三类模式Top15.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eyetracking\各周周报\数据相关\21.04.14-Sequential_Pattern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eyetracking\sequential-pattern-mining-for-eye-track\21.04.14-Sequential_Pattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
   <si>
     <t>Statement; Diagram</t>
   </si>
@@ -152,45 +152,13 @@
     <t>Diagram-&gt;Statement-&gt;Diagram-&gt;Statement-&gt;Diagram</t>
   </si>
   <si>
-    <t>OptionA-&gt;OptionB</t>
-  </si>
-  <si>
     <t>OptionB-&gt;OptionC</t>
   </si>
   <si>
-    <t>OptionC-&gt;OptionB</t>
-  </si>
-  <si>
     <t>OptionA-&gt;OptionC</t>
   </si>
   <si>
     <t>OptionB-&gt;OptionC-&gt;OptionA-&gt;Statement-&gt;Diagram</t>
-  </si>
-  <si>
-    <t>OptionB-&gt;OptionC-&gt;OptionA-&gt;Statement</t>
-  </si>
-  <si>
-    <t>OptionC-&gt;OptionA-&gt;Statement-&gt;Diagram</t>
-  </si>
-  <si>
-    <t>OptionB-&gt;OptionC-&gt;OptionA</t>
-  </si>
-  <si>
-    <t>OptionC-&gt;OptionA-&gt;Statement</t>
-  </si>
-  <si>
-    <t>OptionA-&gt;Statement-&gt;Diagram</t>
-  </si>
-  <si>
-    <t>OptionC-&gt;OptionD</t>
-  </si>
-  <si>
-    <t>Statement-&gt;OptionA</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diagram-&gt;Statement-&gt;Diagram-&gt;Statement</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>correct</t>
@@ -329,10 +297,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>OptionB-&gt;OptionC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>OptionB-&gt;OptionC; OptionC-&gt;OptionA; Statement-&gt;Diagram</t>
   </si>
   <si>
@@ -411,27 +375,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>OptionA-&gt;Statement</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>不连续2-5 length(3331)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>连续2-5 length(960)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> length(2530)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> length(144107)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> length(474)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -442,6 +394,219 @@
     <t>1. Statement和Diagram之前频繁跳转，很可能图和题干离得太近难以区分，实际一直看图的可能性较大。
 2. 从题干到选项的模式二者都有，按部就班的按顺序做题。
 3. 答错者出现选项返回图的模式较多，而答对者没有，可能是看了题之后没有思路去看选项再去看图。答对者几乎都是题干到选项的模式，可能看了一遍图之后就有了答案。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Statement-&gt;Diagram; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Diagram-&gt;Statement; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Statement-&gt;Diagram; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Statement-&gt;Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Statement-&gt;Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>内部变长2-3 length(237363)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Diagram-&gt;Statement-&gt;Diagram; Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>length(133796)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram-&gt;Statement; Diagram-&gt;Statement-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>Statement-&gt;Diagram; Diagram-&gt;Statement; OptionB-&gt;OptionA</t>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; OptionB-&gt;OptionA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement-&gt;Diagram; Diagram-&gt;Statement; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement-&gt;Diagram; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Diagram-&gt;Statement; Statement-&gt;Diagram; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Diagram-&gt;Statement; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Statement-&gt;Diagram</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>OptionB-&gt;OptionC;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> OptionA-&gt;Statement</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement-&gt;Diagram; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Statement-&gt;OptionA</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement-&gt;Diagram; Diagram-&gt;Statement; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Statement-&gt;OptionA</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diagram-&gt;Statement; Statement-&gt;Diagram; OptionB-&gt;OptionA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续2-5 length(985)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> length(476)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OptionA-&gt;OptionC-&gt;Diagram</t>
+  </si>
+  <si>
+    <t>OptionA-&gt;Statement</t>
+  </si>
+  <si>
+    <t>Statement-&gt;OptionA</t>
+  </si>
+  <si>
+    <t>OptionA-&gt;Statement-&gt;Diagram-&gt;Statement</t>
+  </si>
+  <si>
+    <t>这两个只出现在一个人的模式中</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -449,7 +614,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +669,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,12 +686,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,12 +715,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -568,7 +727,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,7 +770,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -609,6 +792,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -621,12 +810,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -636,29 +819,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -945,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:G32"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -959,10 +1146,10 @@
     <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="85.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="85.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47.5546875" bestFit="1" customWidth="1"/>
@@ -973,9 +1160,9 @@
     <col min="18" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>15</v>
@@ -993,7 +1180,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>15</v>
@@ -1011,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>15</v>
@@ -1029,32 +1216,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
       <c r="M2" s="15" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="O2" s="14"/>
       <c r="P2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1091,26 +1278,27 @@
       <c r="L3" s="14">
         <v>0.90828745307380365</v>
       </c>
-      <c r="M3" s="17" t="s">
-        <v>32</v>
+      <c r="M3" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="N3" s="14">
         <v>2</v>
       </c>
       <c r="O3" s="14">
-        <v>6.3452072525633518</v>
-      </c>
-      <c r="P3" s="17" t="s">
+        <v>7.0054109270461797</v>
+      </c>
+      <c r="P3" s="14" t="s">
         <v>33</v>
       </c>
       <c r="Q3" s="14">
         <v>2</v>
       </c>
       <c r="R3" s="14">
-        <v>1.634178391126565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1.9874388382884081</v>
+      </c>
+      <c r="S3" s="13"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1147,26 +1335,27 @@
       <c r="L4" s="14">
         <v>0.69410215067658609</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>33</v>
+      <c r="M4" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="N4" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O4" s="14">
-        <v>5.7942461462181916</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>32</v>
+        <v>6.758435348565885</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="Q4" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4" s="14">
-        <v>1.2322306305356481</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1.8088176336279651</v>
+      </c>
+      <c r="S4" s="13"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1186,7 +1375,7 @@
         <v>0.67828100000000002</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H5" s="14">
         <v>3</v>
@@ -1203,26 +1392,27 @@
       <c r="L5" s="14">
         <v>0.35620869070022748</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>34</v>
+      <c r="M5" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="N5" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="14">
-        <v>5.2550492857484086</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>34</v>
+        <v>6.4616548439921866</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="Q5" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="14">
-        <v>0.97852729189923249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1.503969760970431</v>
+      </c>
+      <c r="S5" s="13"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1259,26 +1449,27 @@
       <c r="L6" s="14">
         <v>0.32764489411800879</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="14" t="s">
         <v>35</v>
       </c>
       <c r="N6" s="14">
         <v>3</v>
       </c>
       <c r="O6" s="14">
-        <v>4.5583352627553246</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>37</v>
+        <v>4.7151434188184558</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="Q6" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R6" s="14">
-        <v>0.86624065311298182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1.3667703163926459</v>
+      </c>
+      <c r="S6" s="13"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
@@ -1315,26 +1506,32 @@
       <c r="L7" s="14">
         <v>0.31759466565942462</v>
       </c>
-      <c r="M7" s="24" t="s">
-        <v>52</v>
+      <c r="M7" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="N7" s="14">
         <v>4</v>
       </c>
       <c r="O7" s="14">
-        <v>4.3069983285585263</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>35</v>
+        <v>4.3676860968744631</v>
+      </c>
+      <c r="P7" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="Q7" s="14">
         <v>3</v>
       </c>
       <c r="R7" s="14">
-        <v>0.80881763362796466</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="S7" s="13">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1353,8 +1550,8 @@
       <c r="F8" s="4">
         <v>0.59458699999999998</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>67</v>
+      <c r="G8" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="H8" s="14">
         <v>3</v>
@@ -1371,27 +1568,28 @@
       <c r="L8" s="14">
         <v>0.31195033736506278</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="14" t="s">
         <v>37</v>
       </c>
       <c r="N8" s="14">
         <v>4</v>
       </c>
       <c r="O8" s="14">
-        <v>3.9728932681266431</v>
+        <v>4.1728932681266429</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R8" s="14">
-        <v>0.79658993095847919</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+        <v>0.98792751362344156</v>
+      </c>
+      <c r="S8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2">
@@ -1409,8 +1607,8 @@
       <c r="F9" s="4">
         <v>0.53974599999999995</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>66</v>
+      <c r="G9" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="H9" s="14">
         <v>3</v>
@@ -1427,26 +1625,27 @@
       <c r="L9" s="14">
         <v>0.30895257911907359</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="N9" s="14">
         <v>5</v>
       </c>
       <c r="O9" s="14">
-        <v>3.801321841824195</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>38</v>
+        <v>3.858258804033591</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="Q9" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R9" s="14">
-        <v>0.7113002946885304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.87010662840565201</v>
+      </c>
+      <c r="S9" s="13"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
@@ -1483,26 +1682,27 @@
       <c r="L10" s="14">
         <v>0.28134384961767323</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="14" t="s">
         <v>39</v>
       </c>
       <c r="N10" s="14">
         <v>5</v>
       </c>
       <c r="O10" s="14">
-        <v>3.4835561124301528</v>
-      </c>
-      <c r="P10" s="22" t="s">
-        <v>39</v>
+        <v>3.7324145599187379</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="Q10" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R10" s="14">
-        <v>0.59682490245266684</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.86624065311298182</v>
+      </c>
+      <c r="S10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1731,7 @@
         <v>1.5524866964849939</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="K11" s="14">
         <v>3</v>
@@ -1540,25 +1740,26 @@
         <v>0.2658469676264773</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="N11" s="14">
         <v>2</v>
       </c>
       <c r="O11" s="14">
-        <v>1.9989439067485779</v>
-      </c>
-      <c r="P11" s="24" t="s">
-        <v>36</v>
+        <v>2.0204699956327241</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="Q11" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R11" s="14">
-        <v>0.57673928146687636</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.79658993095847919</v>
+      </c>
+      <c r="S11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1788,7 @@
         <v>1.5506532155413351</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="K12" s="14">
         <v>3</v>
@@ -1596,27 +1797,28 @@
         <v>0.26449177198508789</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="N12" s="14">
         <v>2</v>
       </c>
       <c r="O12" s="14">
-        <v>1.7798212670636251</v>
+        <v>1.782584998204096</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="14">
         <v>5</v>
       </c>
       <c r="R12" s="14">
-        <v>0.53879310344827591</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.59682490245266684</v>
+      </c>
+      <c r="S12" s="13"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B13" s="14">
         <v>2</v>
@@ -1625,7 +1827,7 @@
         <v>2.5370197222555628</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E13" s="14">
         <v>2</v>
@@ -1634,7 +1836,7 @@
         <v>0.50129975334310251</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H13" s="14">
         <v>3</v>
@@ -1643,7 +1845,7 @@
         <v>1.5443329353539159</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K13" s="14">
         <v>3</v>
@@ -1651,28 +1853,31 @@
       <c r="L13" s="14">
         <v>0.26379338937153402</v>
       </c>
-      <c r="M13" s="26" t="s">
-        <v>68</v>
+      <c r="M13" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="N13" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O13" s="14">
-        <v>1.505021314362704</v>
-      </c>
-      <c r="P13" s="26" t="s">
-        <v>41</v>
+        <v>1.5619750782615469</v>
+      </c>
+      <c r="P13" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="Q13" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R13" s="14">
-        <v>0.49398806931041223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.53879310344827591</v>
+      </c>
+      <c r="S13" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B14" s="14">
         <v>2</v>
@@ -1681,7 +1886,7 @@
         <v>2.534315390024013</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E14" s="14">
         <v>3</v>
@@ -1690,7 +1895,7 @@
         <v>0.48895612425325152</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H14" s="14">
         <v>2</v>
@@ -1699,7 +1904,7 @@
         <v>1.492406050357368</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K14" s="14">
         <v>3</v>
@@ -1707,28 +1912,29 @@
       <c r="L14" s="14">
         <v>0.26337662804336609</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="17" t="s">
         <v>40</v>
       </c>
       <c r="N14" s="14">
         <v>2</v>
       </c>
       <c r="O14" s="14">
-        <v>1.3471416968380581</v>
-      </c>
-      <c r="P14" s="14" t="s">
-        <v>45</v>
+        <v>1.5373877299917551</v>
+      </c>
+      <c r="P14" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="Q14" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R14" s="14">
-        <v>0.44261300920695518</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.49952327031626609</v>
+      </c>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B15" s="14">
         <v>3</v>
@@ -1737,7 +1943,7 @@
         <v>2.5060224029131999</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E15" s="14">
         <v>2</v>
@@ -1746,7 +1952,7 @@
         <v>0.48679020207962609</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H15" s="14">
         <v>2</v>
@@ -1754,8 +1960,8 @@
       <c r="I15" s="14">
         <v>1.492324982648795</v>
       </c>
-      <c r="J15" s="19" t="s">
-        <v>75</v>
+      <c r="J15" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="K15" s="14">
         <v>3</v>
@@ -1763,28 +1969,16 @@
       <c r="L15" s="14">
         <v>0.26314954552750353</v>
       </c>
-      <c r="M15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" s="14">
-        <v>3</v>
-      </c>
-      <c r="O15" s="14">
-        <v>1.263454701839555</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q15" s="14">
-        <v>4</v>
-      </c>
-      <c r="R15" s="14">
-        <v>0.3448687292000493</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B16" s="14">
         <v>3</v>
@@ -1793,7 +1987,7 @@
         <v>2.4558593203926051</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E16" s="14">
         <v>3</v>
@@ -1811,7 +2005,7 @@
         <v>1.454411297182467</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="K16" s="14">
         <v>3</v>
@@ -1819,28 +2013,16 @@
       <c r="L16" s="14">
         <v>0.25304995165063199</v>
       </c>
-      <c r="M16" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" s="14">
-        <v>2</v>
-      </c>
-      <c r="O16" s="14">
-        <v>1.209665741705906</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q16" s="14">
-        <v>3</v>
-      </c>
-      <c r="R16" s="14">
-        <v>0.34332688588007743</v>
-      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B17" s="14">
         <v>3</v>
@@ -1848,7 +2030,7 @@
       <c r="C17" s="14">
         <v>2.2383092913307192</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="14">
@@ -1858,7 +2040,7 @@
         <v>0.47495962712815631</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H17" s="14">
         <v>2</v>
@@ -1866,8 +2048,8 @@
       <c r="I17" s="14">
         <v>1.4366143342584019</v>
       </c>
-      <c r="J17" s="21" t="s">
-        <v>76</v>
+      <c r="J17" s="20" t="s">
+        <v>65</v>
       </c>
       <c r="K17" s="14">
         <v>3</v>
@@ -1875,93 +2057,540 @@
       <c r="L17" s="14">
         <v>0.25285635969863762</v>
       </c>
-      <c r="M17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="14">
-        <v>2</v>
-      </c>
-      <c r="O17" s="14">
-        <v>1.1714552662024089</v>
-      </c>
-      <c r="P17" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q17" s="14">
-        <v>3</v>
-      </c>
-      <c r="R17" s="14">
-        <v>0.32633806554067168</v>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G18" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="14">
+        <v>2</v>
+      </c>
+      <c r="I19" s="14">
+        <v>10.369672629349081</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="14">
+        <v>2</v>
+      </c>
+      <c r="L19" s="14">
+        <v>1.8291436745431811</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="14">
+        <v>2</v>
+      </c>
+      <c r="I20" s="14">
+        <v>9.9837030470700689</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="14">
+        <v>2</v>
+      </c>
+      <c r="L20" s="14">
+        <v>1.7702340115036761</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="14">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14">
+        <v>7.0194432553594739</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" s="14">
+        <v>2</v>
+      </c>
+      <c r="L21" s="14">
+        <v>1.254915255844161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="14">
+        <v>2</v>
+      </c>
+      <c r="I22" s="14">
+        <v>6.8954665767754184</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" s="14">
+        <v>2</v>
+      </c>
+      <c r="L22" s="14">
+        <v>1.1916206862018039</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G23" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="14">
+        <v>2</v>
+      </c>
+      <c r="I23" s="14">
+        <v>6.5087938694061194</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K23" s="14">
+        <v>2</v>
+      </c>
+      <c r="L23" s="14">
+        <v>1.1911630905887529</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G24" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="14">
+        <v>3</v>
+      </c>
+      <c r="I24" s="14">
+        <v>6.3374670597954088</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="14">
+        <v>3</v>
+      </c>
+      <c r="L24" s="14">
+        <v>1.153263619814576</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G25" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="14">
+        <v>3</v>
+      </c>
+      <c r="I25" s="14">
+        <v>6.3217694619766851</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25" s="14">
+        <v>2</v>
+      </c>
+      <c r="L25" s="14">
+        <v>1.1468643407773931</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="14">
+        <v>2</v>
+      </c>
+      <c r="I26" s="14">
+        <v>6.2760312643310536</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K26" s="14">
+        <v>3</v>
+      </c>
+      <c r="L26" s="14">
+        <v>1.143854157411508</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="14">
+        <v>3</v>
+      </c>
+      <c r="I27" s="14">
+        <v>5.9836934057446136</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="14">
+        <v>3</v>
+      </c>
+      <c r="L27" s="14">
+        <v>1.094757422188813</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="14">
+        <v>3</v>
+      </c>
+      <c r="I28" s="14">
+        <v>5.9383908678099777</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="14">
+        <v>3</v>
+      </c>
+      <c r="L28" s="14">
+        <v>1.089819324998563</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="14">
+        <v>3</v>
+      </c>
+      <c r="I29" s="14">
+        <v>4.3897596270999717</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K29" s="14">
+        <v>3</v>
+      </c>
+      <c r="L29" s="14">
+        <v>0.90419710971452649</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="14">
+        <v>2</v>
+      </c>
+      <c r="I30" s="14">
+        <v>4.3613128443212368</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K30" s="14">
+        <v>3</v>
+      </c>
+      <c r="L30" s="14">
+        <v>0.85522039913159154</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="14">
+        <v>3</v>
+      </c>
+      <c r="I31" s="14">
+        <v>4.3610149116203862</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="K31" s="14">
+        <v>2</v>
+      </c>
+      <c r="L31" s="14">
+        <v>0.82518947104916163</v>
+      </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="14">
+        <v>3</v>
+      </c>
+      <c r="I32" s="14">
+        <v>4.3411222434093766</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="14">
+        <v>2</v>
+      </c>
+      <c r="L32" s="14">
+        <v>0.7666684039521714</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" s="14">
+        <v>3</v>
+      </c>
+      <c r="I33" s="14">
+        <v>4.3117269414658388</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" s="14">
+        <v>3</v>
+      </c>
+      <c r="L33" s="14">
+        <v>0.74423342932125014</v>
+      </c>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G34" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" s="14">
+        <v>3</v>
+      </c>
+      <c r="I34" s="14">
+        <v>4.2962083756713909</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="K34" s="14">
+        <v>2</v>
+      </c>
+      <c r="L34" s="14">
+        <v>0.71680253268298499</v>
+      </c>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G35" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="14">
+        <v>2</v>
+      </c>
+      <c r="I35" s="14">
+        <v>4.1528259547842064</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="K35" s="14">
+        <v>2</v>
+      </c>
+      <c r="L35" s="14">
+        <v>0.71203914489357101</v>
+      </c>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G36" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H36" s="14">
+        <v>2</v>
+      </c>
+      <c r="I36" s="14">
+        <v>4.1282633095097072</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="K36" s="14">
+        <v>3</v>
+      </c>
+      <c r="L36" s="14">
+        <v>0.70948649937441022</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G37" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H37" s="14">
+        <v>3</v>
+      </c>
+      <c r="I37" s="14">
+        <v>4.0941451675397733</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37" s="14">
+        <v>3</v>
+      </c>
+      <c r="L37" s="14">
+        <v>0.70640597292240015</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G38" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" s="14">
+        <v>3</v>
+      </c>
+      <c r="I38" s="14">
+        <v>4.0937049549303186</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K38" s="14">
+        <v>2</v>
+      </c>
+      <c r="L38" s="14">
+        <v>0.68165129054982432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A27:G32"/>
+    <mergeCell ref="A39:G45"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>